<commit_message>
only measure encoding and solving time of cpsat & rerun
</commit_message>
<xml_diff>
--- a/other-approaches/CPSAT/nrp_cpsat_exp_results.xlsx
+++ b/other-approaches/CPSAT/nrp_cpsat_exp_results.xlsx
@@ -472,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.106</v>
+        <v>0.112</v>
       </c>
       <c r="F2" t="n">
-        <v>16.49</v>
+        <v>17.04</v>
       </c>
     </row>
     <row r="3">
@@ -494,10 +494,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.057</v>
+        <v>0.055</v>
       </c>
       <c r="F3" t="n">
-        <v>17.07</v>
+        <v>17.18</v>
       </c>
     </row>
     <row r="4">
@@ -516,10 +516,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.047</v>
+        <v>0.055</v>
       </c>
       <c r="F4" t="n">
-        <v>16.64</v>
+        <v>17.18</v>
       </c>
     </row>
     <row r="5">
@@ -538,10 +538,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.055</v>
+        <v>0.052</v>
       </c>
       <c r="F5" t="n">
-        <v>17.21</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
         <v>0.054</v>
       </c>
       <c r="F6" t="n">
-        <v>17.09</v>
+        <v>17.29</v>
       </c>
     </row>
     <row r="7">
@@ -582,10 +582,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05</v>
+        <v>0.049</v>
       </c>
       <c r="F7" t="n">
-        <v>16.83</v>
+        <v>16.95</v>
       </c>
     </row>
     <row r="8">
@@ -604,10 +604,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.047</v>
+        <v>0.053</v>
       </c>
       <c r="F8" t="n">
-        <v>16.63</v>
+        <v>17.12</v>
       </c>
     </row>
     <row r="9">
@@ -626,10 +626,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.053</v>
+        <v>0.054</v>
       </c>
       <c r="F9" t="n">
-        <v>16.93</v>
+        <v>17.07</v>
       </c>
     </row>
     <row r="10">
@@ -648,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.047</v>
+        <v>0.053</v>
       </c>
       <c r="F10" t="n">
-        <v>16.63</v>
+        <v>17.01</v>
       </c>
     </row>
     <row r="11">
@@ -670,10 +670,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.049</v>
+        <v>0.055</v>
       </c>
       <c r="F11" t="n">
-        <v>16.85</v>
+        <v>17.11</v>
       </c>
     </row>
     <row r="12">
@@ -690,10 +690,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.05650000000000001</v>
+        <v>0.05920000000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>16.837</v>
+        <v>17.075</v>
       </c>
     </row>
   </sheetData>
@@ -763,10 +763,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.078</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>19.1</v>
+        <v>19.27</v>
       </c>
     </row>
     <row r="3">
@@ -785,10 +785,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08</v>
+        <v>0.083</v>
       </c>
       <c r="F3" t="n">
-        <v>19.11</v>
+        <v>18.89</v>
       </c>
     </row>
     <row r="4">
@@ -807,10 +807,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.08</v>
+        <v>0.083</v>
       </c>
       <c r="F4" t="n">
-        <v>19.07</v>
+        <v>18.86</v>
       </c>
     </row>
     <row r="5">
@@ -829,10 +829,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.079</v>
+        <v>0.083</v>
       </c>
       <c r="F5" t="n">
-        <v>18.99</v>
+        <v>19.19</v>
       </c>
     </row>
     <row r="6">
@@ -851,10 +851,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.08</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>18.31</v>
+        <v>18.94</v>
       </c>
     </row>
     <row r="7">
@@ -873,10 +873,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.082</v>
+        <v>0.081</v>
       </c>
       <c r="F7" t="n">
-        <v>19.4</v>
+        <v>19.14</v>
       </c>
     </row>
     <row r="8">
@@ -895,10 +895,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.08</v>
+        <v>0.079</v>
       </c>
       <c r="F8" t="n">
-        <v>18.81</v>
+        <v>18.97</v>
       </c>
     </row>
     <row r="9">
@@ -917,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.081</v>
+        <v>0.083</v>
       </c>
       <c r="F9" t="n">
-        <v>19.04</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="10">
@@ -939,10 +939,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.082</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="F10" t="n">
-        <v>19.37</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="11">
@@ -961,10 +961,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.083</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="F11" t="n">
-        <v>19.12</v>
+        <v>19.77</v>
       </c>
     </row>
     <row r="12">
@@ -981,10 +981,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.08049999999999999</v>
+        <v>0.08309999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>19.032</v>
+        <v>19.098</v>
       </c>
     </row>
   </sheetData>
@@ -1057,7 +1057,7 @@
         <v>0.138</v>
       </c>
       <c r="F2" t="n">
-        <v>25.99</v>
+        <v>26.01</v>
       </c>
     </row>
     <row r="3">
@@ -1076,10 +1076,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.137</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>26.06</v>
+        <v>25.95</v>
       </c>
     </row>
     <row r="4">
@@ -1098,10 +1098,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.135</v>
+        <v>0.14</v>
       </c>
       <c r="F4" t="n">
-        <v>26.03</v>
+        <v>26.02</v>
       </c>
     </row>
     <row r="5">
@@ -1120,10 +1120,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.136</v>
+        <v>0.141</v>
       </c>
       <c r="F5" t="n">
-        <v>25.93</v>
+        <v>26.04</v>
       </c>
     </row>
     <row r="6">
@@ -1142,10 +1142,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.134</v>
+        <v>0.139</v>
       </c>
       <c r="F6" t="n">
-        <v>25.96</v>
+        <v>26.06</v>
       </c>
     </row>
     <row r="7">
@@ -1164,10 +1164,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.131</v>
+        <v>0.139</v>
       </c>
       <c r="F7" t="n">
-        <v>25.88</v>
+        <v>25.91</v>
       </c>
     </row>
     <row r="8">
@@ -1186,10 +1186,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.139</v>
+        <v>0.141</v>
       </c>
       <c r="F8" t="n">
-        <v>25.96</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -1208,10 +1208,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.139</v>
+        <v>0.141</v>
       </c>
       <c r="F9" t="n">
-        <v>25.9</v>
+        <v>26.08</v>
       </c>
     </row>
     <row r="10">
@@ -1233,7 +1233,7 @@
         <v>0.139</v>
       </c>
       <c r="F10" t="n">
-        <v>25.98</v>
+        <v>25.96</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.136</v>
+        <v>0.138</v>
       </c>
       <c r="F11" t="n">
-        <v>26</v>
+        <v>25.98</v>
       </c>
     </row>
     <row r="12">
@@ -1272,10 +1272,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.1364</v>
+        <v>0.1396</v>
       </c>
       <c r="F12" t="n">
-        <v>25.96899999999999</v>
+        <v>26.001</v>
       </c>
     </row>
   </sheetData>
@@ -1345,10 +1345,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.142</v>
+        <v>0.148</v>
       </c>
       <c r="F2" t="n">
-        <v>28.02</v>
+        <v>29.62</v>
       </c>
     </row>
     <row r="3">
@@ -1367,10 +1367,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.144</v>
       </c>
       <c r="F3" t="n">
-        <v>29.64</v>
+        <v>29.57</v>
       </c>
     </row>
     <row r="4">
@@ -1389,10 +1389,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0.141</v>
+        <v>0.15</v>
       </c>
       <c r="F4" t="n">
-        <v>29.74</v>
+        <v>31.18</v>
       </c>
     </row>
     <row r="5">
@@ -1411,10 +1411,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0.14</v>
+        <v>0.146</v>
       </c>
       <c r="F5" t="n">
-        <v>29.78</v>
+        <v>29.51</v>
       </c>
     </row>
     <row r="6">
@@ -1433,10 +1433,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.143</v>
+        <v>0.148</v>
       </c>
       <c r="F6" t="n">
-        <v>31.54</v>
+        <v>29.72</v>
       </c>
     </row>
     <row r="7">
@@ -1455,10 +1455,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.141</v>
+        <v>0.148</v>
       </c>
       <c r="F7" t="n">
-        <v>31.48</v>
+        <v>31.43</v>
       </c>
     </row>
     <row r="8">
@@ -1477,10 +1477,10 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>0.141</v>
+        <v>0.149</v>
       </c>
       <c r="F8" t="n">
-        <v>29.63</v>
+        <v>29.77</v>
       </c>
     </row>
     <row r="9">
@@ -1499,10 +1499,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>0.143</v>
+        <v>0.149</v>
       </c>
       <c r="F9" t="n">
-        <v>29.8</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="10">
@@ -1521,10 +1521,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>0.142</v>
+        <v>0.147</v>
       </c>
       <c r="F10" t="n">
-        <v>29.59</v>
+        <v>29.34</v>
       </c>
     </row>
     <row r="11">
@@ -1543,10 +1543,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>0.14</v>
+        <v>0.149</v>
       </c>
       <c r="F11" t="n">
-        <v>29.79</v>
+        <v>29.56</v>
       </c>
     </row>
     <row r="12">
@@ -1563,10 +1563,10 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.1413</v>
+        <v>0.1478</v>
       </c>
       <c r="F12" t="n">
-        <v>29.901</v>
+        <v>29.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>